<commit_message>
Add Expenditure Update 12
</commit_message>
<xml_diff>
--- a/Civilworks cost/output.xlsx
+++ b/Civilworks cost/output.xlsx
@@ -12736,8 +12736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="L63" sqref="L63"/>
     </sheetView>

</xml_diff>

<commit_message>
civil work cost update
</commit_message>
<xml_diff>
--- a/Civilworks cost/output.xlsx
+++ b/Civilworks cost/output.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="original" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="248">
   <si>
     <t xml:space="preserve">Sl No </t>
   </si>
@@ -766,6 +766,9 @@
   <si>
     <t>GT-03</t>
   </si>
+  <si>
+    <t xml:space="preserve">251/(SUNM-02)-02  4th RA Bill </t>
+  </si>
 </sst>
 </file>
 
@@ -12736,10 +12739,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="D1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="H1" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="L63" sqref="L63"/>
+      <selection pane="bottomLeft" activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12750,7 +12753,8 @@
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.21875" style="2" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" customWidth="1"/>
-    <col min="8" max="9" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.109375" customWidth="1"/>
+    <col min="9" max="9" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.5546875" customWidth="1"/>
     <col min="12" max="12" width="16.109375" customWidth="1"/>
@@ -15466,7 +15470,7 @@
         <v>0</v>
       </c>
       <c r="C52" t="s">
-        <v>68</v>
+        <v>247</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -18271,16 +18275,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L63" sqref="L63"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="30.33203125" customWidth="1"/>
     <col min="7" max="7" width="17.21875" customWidth="1"/>
+    <col min="8" max="8" width="13.5546875" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" customWidth="1"/>
     <col min="11" max="11" width="22" customWidth="1"/>
+    <col min="12" max="12" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.3">
@@ -20991,7 +20998,7 @@
         <v>0</v>
       </c>
       <c r="C52" t="s">
-        <v>68</v>
+        <v>247</v>
       </c>
       <c r="D52">
         <v>0</v>

</xml_diff>

<commit_message>
Server Setup commandas update
</commit_message>
<xml_diff>
--- a/Civilworks cost/output.xlsx
+++ b/Civilworks cost/output.xlsx
@@ -18913,3701 +18913,3286 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I142"/>
+  <dimension ref="A1:H142"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="4" max="4" width="23.44140625" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="10" max="10" width="21.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>201</v>
+      </c>
       <c r="B1" s="1" t="s">
-        <v>201</v>
+        <v>14</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>202</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>202</v>
+        <v>15</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>13</v>
+        <v>203</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="I1" s="1" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>0</v>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B2">
+        <v>394997.96</v>
       </c>
       <c r="C2">
-        <v>394997.96</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>2426416.04</v>
       </c>
       <c r="E2">
-        <v>2426416.04</v>
+        <v>2821414</v>
       </c>
       <c r="F2">
-        <v>2821414</v>
-      </c>
-      <c r="G2">
         <v>404</v>
       </c>
-      <c r="H2" t="s">
+      <c r="G2" t="s">
         <v>206</v>
       </c>
-      <c r="I2">
+      <c r="H2">
         <v>3632</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>1</v>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>99178.53</v>
       </c>
       <c r="C3">
-        <v>99178.53</v>
+        <v>0</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>609239.1100000001</v>
       </c>
       <c r="E3">
-        <v>609239.1100000001</v>
+        <v>708417.64000000013</v>
       </c>
       <c r="F3">
-        <v>708417.64000000013</v>
-      </c>
-      <c r="G3">
         <v>404</v>
       </c>
-      <c r="H3" t="s">
+      <c r="G3" t="s">
         <v>207</v>
       </c>
-      <c r="I3">
+      <c r="H3">
         <v>3682</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>2</v>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>10674.86</v>
       </c>
       <c r="C4">
-        <v>10674.86</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>65574.149999999994</v>
       </c>
       <c r="E4">
-        <v>65574.149999999994</v>
+        <v>76249.009999999995</v>
       </c>
       <c r="F4">
-        <v>76249.009999999995</v>
-      </c>
-      <c r="G4">
         <v>405</v>
       </c>
-      <c r="H4" t="s">
+      <c r="G4" t="s">
         <v>207</v>
       </c>
-      <c r="I4">
+      <c r="H4">
         <v>3682</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>3</v>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>120439.61</v>
       </c>
       <c r="C5">
-        <v>120439.61</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>739842.74000000011</v>
       </c>
       <c r="E5">
-        <v>739842.74000000011</v>
+        <v>860282.35000000009</v>
       </c>
       <c r="F5">
-        <v>860282.35000000009</v>
-      </c>
-      <c r="G5">
         <v>409</v>
       </c>
-      <c r="H5" t="s">
+      <c r="G5" t="s">
         <v>207</v>
       </c>
-      <c r="I5">
+      <c r="H5">
         <v>3682</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>4</v>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>1107145</v>
       </c>
       <c r="C6">
-        <v>1107145</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>6801038.2400000002</v>
       </c>
       <c r="E6">
-        <v>6801038.2400000002</v>
+        <v>7908183.2400000002</v>
       </c>
       <c r="F6">
-        <v>7908183.2400000002</v>
-      </c>
-      <c r="G6">
         <v>404</v>
       </c>
-      <c r="H6" t="s">
+      <c r="G6" t="s">
         <v>208</v>
       </c>
-      <c r="I6">
+      <c r="H6">
         <v>3700</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>5</v>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>474759.39</v>
       </c>
       <c r="C7">
-        <v>474759.39</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>2916378.91</v>
       </c>
       <c r="E7">
-        <v>2916378.91</v>
+        <v>3391138.3</v>
       </c>
       <c r="F7">
-        <v>3391138.3</v>
-      </c>
-      <c r="G7">
         <v>404</v>
       </c>
-      <c r="H7" t="s">
+      <c r="G7" t="s">
         <v>208</v>
       </c>
-      <c r="I7">
+      <c r="H7">
         <v>3701</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>6</v>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>1212067.8500000001</v>
       </c>
       <c r="C8">
-        <v>1212067.8500000001</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>7445559.0899999999</v>
       </c>
       <c r="E8">
-        <v>7445559.0899999999</v>
+        <v>8657626.9399999995</v>
       </c>
       <c r="F8">
-        <v>8657626.9399999995</v>
-      </c>
-      <c r="G8">
         <v>405</v>
       </c>
-      <c r="H8" t="s">
+      <c r="G8" t="s">
         <v>208</v>
       </c>
-      <c r="I8">
+      <c r="H8">
         <v>3701</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>7</v>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>134870.79999999999</v>
       </c>
       <c r="C9">
-        <v>134870.79999999999</v>
+        <v>0</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>828492.04</v>
       </c>
       <c r="E9">
-        <v>828492.04</v>
+        <v>963362.84000000008</v>
       </c>
       <c r="F9">
-        <v>963362.84000000008</v>
-      </c>
-      <c r="G9">
         <v>402</v>
       </c>
-      <c r="H9" t="s">
+      <c r="G9" t="s">
         <v>209</v>
       </c>
-      <c r="I9">
+      <c r="H9">
         <v>3707</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>8</v>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>363410.06</v>
       </c>
       <c r="C10">
-        <v>363410.06</v>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>2232376.1</v>
       </c>
       <c r="E10">
-        <v>2232376.1</v>
+        <v>2595786.16</v>
       </c>
       <c r="F10">
-        <v>2595786.16</v>
-      </c>
-      <c r="G10">
         <v>404</v>
       </c>
-      <c r="H10" t="s">
+      <c r="G10" t="s">
         <v>209</v>
       </c>
-      <c r="I10">
+      <c r="H10">
         <v>3707</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>9</v>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>1227017.96</v>
       </c>
       <c r="C11">
-        <v>1227017.96</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>7537396.04</v>
       </c>
       <c r="E11">
-        <v>7537396.04</v>
+        <v>8764414</v>
       </c>
       <c r="F11">
-        <v>8764414</v>
-      </c>
-      <c r="G11">
         <v>409</v>
       </c>
-      <c r="H11" t="s">
+      <c r="G11" t="s">
         <v>209</v>
       </c>
-      <c r="I11">
+      <c r="H11">
         <v>3707</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
-        <v>10</v>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>1804397.95</v>
       </c>
       <c r="C12">
-        <v>1804397.95</v>
+        <v>0</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>11084158.84</v>
       </c>
       <c r="E12">
-        <v>11084158.84</v>
+        <v>12888556.789999999</v>
       </c>
       <c r="F12">
-        <v>12888556.789999999</v>
-      </c>
-      <c r="G12">
         <v>404</v>
       </c>
-      <c r="H12" t="s">
+      <c r="G12" t="s">
         <v>210</v>
       </c>
-      <c r="I12">
+      <c r="H12">
         <v>3729</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
-        <v>11</v>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>923233.39</v>
       </c>
       <c r="C13">
-        <v>923233.39</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>5671290.8200000003</v>
       </c>
       <c r="E13">
-        <v>5671290.8200000003</v>
+        <v>6594524.21</v>
       </c>
       <c r="F13">
-        <v>6594524.21</v>
-      </c>
-      <c r="G13">
         <v>405</v>
       </c>
-      <c r="H13" t="s">
+      <c r="G13" t="s">
         <v>210</v>
       </c>
-      <c r="I13">
+      <c r="H13">
         <v>3729</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
-        <v>12</v>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>4651.5</v>
       </c>
       <c r="C14">
-        <v>4651.5</v>
+        <v>0</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>28573.5</v>
       </c>
       <c r="E14">
-        <v>28573.5</v>
+        <v>33225</v>
       </c>
       <c r="F14">
-        <v>33225</v>
-      </c>
-      <c r="G14">
         <v>404</v>
       </c>
-      <c r="H14" t="s">
+      <c r="G14" t="s">
         <v>211</v>
       </c>
-      <c r="I14">
+      <c r="H14">
         <v>3732</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <v>13</v>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>2982</v>
       </c>
       <c r="C15">
-        <v>2982</v>
+        <v>0</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>18318</v>
       </c>
       <c r="E15">
-        <v>18318</v>
+        <v>21300</v>
       </c>
       <c r="F15">
-        <v>21300</v>
-      </c>
-      <c r="G15">
         <v>406</v>
       </c>
-      <c r="H15" t="s">
+      <c r="G15" t="s">
         <v>211</v>
       </c>
-      <c r="I15">
+      <c r="H15">
         <v>3732</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
-        <v>14</v>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>13368.6</v>
       </c>
       <c r="C16">
-        <v>13368.6</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>82121.399999999994</v>
       </c>
       <c r="E16">
-        <v>82121.399999999994</v>
+        <v>95490</v>
       </c>
       <c r="F16">
-        <v>95490</v>
-      </c>
-      <c r="G16">
         <v>408</v>
       </c>
-      <c r="H16" t="s">
+      <c r="G16" t="s">
         <v>211</v>
       </c>
-      <c r="I16">
+      <c r="H16">
         <v>3732</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <v>15</v>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>2989816.9</v>
       </c>
       <c r="C17">
-        <v>2989816.9</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>18366018.100000001</v>
       </c>
       <c r="E17">
-        <v>18366018.100000001</v>
+        <v>21355835</v>
       </c>
       <c r="F17">
-        <v>21355835</v>
-      </c>
-      <c r="G17">
         <v>409</v>
       </c>
-      <c r="H17" t="s">
+      <c r="G17" t="s">
         <v>211</v>
       </c>
-      <c r="I17">
+      <c r="H17">
         <v>3732</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <v>16</v>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>399688.18</v>
       </c>
       <c r="C18">
-        <v>399688.18</v>
+        <v>0</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>2455227.41</v>
       </c>
       <c r="E18">
-        <v>2455227.41</v>
+        <v>2854915.59</v>
       </c>
       <c r="F18">
-        <v>2854915.59</v>
-      </c>
-      <c r="G18">
         <v>404</v>
       </c>
-      <c r="H18" t="s">
+      <c r="G18" t="s">
         <v>212</v>
       </c>
-      <c r="I18">
+      <c r="H18">
         <v>3740</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>17</v>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>1131054.8799999999</v>
       </c>
       <c r="C19">
-        <v>1131054.8799999999</v>
+        <v>0</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>6947908.5300000003</v>
       </c>
       <c r="E19">
-        <v>6947908.5300000003</v>
+        <v>8078963.4100000001</v>
       </c>
       <c r="F19">
-        <v>8078963.4100000001</v>
-      </c>
-      <c r="G19">
         <v>405</v>
       </c>
-      <c r="H19" t="s">
+      <c r="G19" t="s">
         <v>212</v>
       </c>
-      <c r="I19">
+      <c r="H19">
         <v>3740</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>18</v>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>1375509.8</v>
       </c>
       <c r="C20">
-        <v>1375509.8</v>
+        <v>0</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>8449560.1999999993</v>
       </c>
       <c r="E20">
-        <v>8449560.1999999993</v>
+        <v>9825070</v>
       </c>
       <c r="F20">
-        <v>9825070</v>
-      </c>
-      <c r="G20">
         <v>404</v>
       </c>
-      <c r="H20" t="s">
+      <c r="G20" t="s">
         <v>213</v>
       </c>
-      <c r="I20">
+      <c r="H20">
         <v>3754</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>19</v>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>7210009.5199999996</v>
       </c>
       <c r="C21">
-        <v>7210009.5199999996</v>
+        <v>0</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>44290058.479999997</v>
       </c>
       <c r="E21">
-        <v>44290058.479999997</v>
+        <v>51500068</v>
       </c>
       <c r="F21">
-        <v>51500068</v>
-      </c>
-      <c r="G21">
         <v>409</v>
       </c>
-      <c r="H21" t="s">
+      <c r="G21" t="s">
         <v>213</v>
       </c>
-      <c r="I21">
+      <c r="H21">
         <v>3755</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>20</v>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>619590.88</v>
       </c>
       <c r="C22">
-        <v>619590.88</v>
+        <v>0</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>4146492.81</v>
       </c>
       <c r="E22">
-        <v>4146492.81</v>
+        <v>4766083.6900000004</v>
       </c>
       <c r="F22">
-        <v>4766083.6900000004</v>
-      </c>
-      <c r="G22">
         <v>404</v>
       </c>
-      <c r="H22" t="s">
+      <c r="G22" t="s">
         <v>213</v>
       </c>
-      <c r="I22">
+      <c r="H22">
         <v>3757</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="1">
-        <v>21</v>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>156474.93</v>
       </c>
       <c r="C23">
-        <v>156474.93</v>
+        <v>0</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>1047178.38</v>
       </c>
       <c r="E23">
-        <v>1047178.38</v>
+        <v>1203653.31</v>
       </c>
       <c r="F23">
-        <v>1203653.31</v>
-      </c>
-      <c r="G23">
         <v>405</v>
       </c>
-      <c r="H23" t="s">
+      <c r="G23" t="s">
         <v>213</v>
       </c>
-      <c r="I23">
+      <c r="H23">
         <v>3757</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
-        <v>22</v>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>16919.099999999999</v>
       </c>
       <c r="C24">
-        <v>16919.099999999999</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>103931.61</v>
       </c>
       <c r="E24">
-        <v>103931.61</v>
+        <v>120850.71</v>
       </c>
       <c r="F24">
-        <v>120850.71</v>
-      </c>
-      <c r="G24">
         <v>404</v>
       </c>
-      <c r="H24" t="s">
+      <c r="G24" t="s">
         <v>214</v>
       </c>
-      <c r="I24">
+      <c r="H24">
         <v>3761</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="1">
-        <v>23</v>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>36478.06</v>
       </c>
       <c r="C25">
-        <v>36478.06</v>
+        <v>0</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>224079.5</v>
       </c>
       <c r="E25">
-        <v>224079.5</v>
+        <v>260557.56</v>
       </c>
       <c r="F25">
-        <v>260557.56</v>
-      </c>
-      <c r="G25">
         <v>406</v>
       </c>
-      <c r="H25" t="s">
+      <c r="G25" t="s">
         <v>214</v>
       </c>
-      <c r="I25">
+      <c r="H25">
         <v>3761</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="1">
-        <v>24</v>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>3174306.06</v>
       </c>
       <c r="C26">
-        <v>3174306.06</v>
+        <v>0</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>19499308.68</v>
       </c>
       <c r="E26">
-        <v>19499308.68</v>
+        <v>22673614.739999998</v>
       </c>
       <c r="F26">
-        <v>22673614.739999998</v>
-      </c>
-      <c r="G26">
         <v>408</v>
       </c>
-      <c r="H26" t="s">
+      <c r="G26" t="s">
         <v>214</v>
       </c>
-      <c r="I26">
+      <c r="H26">
         <v>3761</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="1">
-        <v>25</v>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>2348428.81</v>
       </c>
       <c r="C27">
-        <v>2348428.81</v>
+        <v>0</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>14426062.689999999</v>
       </c>
       <c r="E27">
-        <v>14426062.689999999</v>
+        <v>16774491.5</v>
       </c>
       <c r="F27">
-        <v>16774491.5</v>
-      </c>
-      <c r="G27">
         <v>404</v>
       </c>
-      <c r="H27" t="s">
+      <c r="G27" t="s">
         <v>214</v>
       </c>
-      <c r="I27">
+      <c r="H27">
         <v>3767</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="1">
-        <v>26</v>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>83743.17</v>
       </c>
       <c r="C28">
-        <v>83743.17</v>
+        <v>0</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>514422.33</v>
       </c>
       <c r="E28">
-        <v>514422.33</v>
+        <v>598165.5</v>
       </c>
       <c r="F28">
-        <v>598165.5</v>
-      </c>
-      <c r="G28">
         <v>405</v>
       </c>
-      <c r="H28" t="s">
+      <c r="G28" t="s">
         <v>214</v>
       </c>
-      <c r="I28">
+      <c r="H28">
         <v>3767</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
-        <v>27</v>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>749535.36</v>
       </c>
       <c r="C29">
-        <v>749535.36</v>
+        <v>0</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>4604288.6399999997</v>
       </c>
       <c r="E29">
-        <v>4604288.6399999997</v>
+        <v>5353824</v>
       </c>
       <c r="F29">
-        <v>5353824</v>
-      </c>
-      <c r="G29">
         <v>409</v>
       </c>
-      <c r="H29" t="s">
+      <c r="G29" t="s">
         <v>215</v>
       </c>
-      <c r="I29">
+      <c r="H29">
         <v>3773</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="1">
-        <v>28</v>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>1009747.2</v>
       </c>
       <c r="C30">
-        <v>1009747.2</v>
+        <v>0</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>6202732.7999999998</v>
       </c>
       <c r="E30">
-        <v>6202732.7999999998</v>
+        <v>7212480</v>
       </c>
       <c r="F30">
-        <v>7212480</v>
-      </c>
-      <c r="G30">
         <v>405</v>
       </c>
-      <c r="H30" t="s">
+      <c r="G30" t="s">
         <v>215</v>
       </c>
-      <c r="I30">
+      <c r="H30">
         <v>3772</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="1">
-        <v>29</v>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>1128992.48</v>
       </c>
       <c r="C31">
-        <v>1128992.48</v>
+        <v>0</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>6935239.5199999996</v>
       </c>
       <c r="E31">
-        <v>6935239.5199999996</v>
+        <v>8064232</v>
       </c>
       <c r="F31">
-        <v>8064232</v>
-      </c>
-      <c r="G31">
         <v>406</v>
       </c>
-      <c r="H31" t="s">
+      <c r="G31" t="s">
         <v>216</v>
       </c>
-      <c r="I31">
+      <c r="H31">
         <v>3781</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="1">
-        <v>30</v>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>2859254.02</v>
       </c>
       <c r="C32">
-        <v>2859254.02</v>
+        <v>0</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>17563988.98</v>
       </c>
       <c r="E32">
-        <v>17563988.98</v>
+        <v>20423243</v>
       </c>
       <c r="F32">
-        <v>20423243</v>
-      </c>
-      <c r="G32">
         <v>408</v>
       </c>
-      <c r="H32" t="s">
+      <c r="G32" t="s">
         <v>216</v>
       </c>
-      <c r="I32">
+      <c r="H32">
         <v>3783</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="1">
-        <v>31</v>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>1544527.88</v>
       </c>
       <c r="C33">
-        <v>1544527.88</v>
+        <v>0</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>9487814.1199999992</v>
       </c>
       <c r="E33">
-        <v>9487814.1199999992</v>
+        <v>11032342</v>
       </c>
       <c r="F33">
-        <v>11032342</v>
-      </c>
-      <c r="G33">
         <v>409</v>
       </c>
-      <c r="H33" t="s">
+      <c r="G33" t="s">
         <v>216</v>
       </c>
-      <c r="I33">
+      <c r="H33">
         <v>3784</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="1">
-        <v>32</v>
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>670690.67000000004</v>
       </c>
       <c r="C34">
-        <v>670690.67000000004</v>
+        <v>0</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>4488468.33</v>
       </c>
       <c r="E34">
-        <v>4488468.33</v>
+        <v>5159159</v>
       </c>
       <c r="F34">
-        <v>5159159</v>
-      </c>
-      <c r="G34">
         <v>409</v>
       </c>
-      <c r="H34" t="s">
+      <c r="G34" t="s">
         <v>217</v>
       </c>
-      <c r="I34">
+      <c r="H34">
         <v>3792</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="1">
-        <v>33</v>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>5141909.92</v>
       </c>
       <c r="C35">
-        <v>5141909.92</v>
+        <v>0</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>31586018</v>
       </c>
       <c r="E35">
-        <v>31586018</v>
+        <v>36727927.920000002</v>
       </c>
       <c r="F35">
-        <v>36727927.920000002</v>
-      </c>
-      <c r="G35">
         <v>409</v>
       </c>
-      <c r="H35" t="s">
+      <c r="G35" t="s">
         <v>218</v>
       </c>
-      <c r="I35">
+      <c r="H35">
         <v>3794</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="1">
-        <v>34</v>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <v>1183.31</v>
       </c>
       <c r="C36">
-        <v>1183.31</v>
+        <v>0</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>7268.89</v>
       </c>
       <c r="E36">
-        <v>7268.89</v>
+        <v>8452.2000000000007</v>
       </c>
       <c r="F36">
-        <v>8452.2000000000007</v>
-      </c>
-      <c r="G36">
         <v>402</v>
       </c>
-      <c r="H36" t="s">
+      <c r="G36" t="s">
         <v>218</v>
       </c>
-      <c r="I36">
+      <c r="H36">
         <v>3793</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="1">
-        <v>35</v>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B37">
+        <v>3240497.81</v>
       </c>
       <c r="C37">
-        <v>3240497.81</v>
+        <v>0</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>19905915.140000001</v>
       </c>
       <c r="E37">
-        <v>19905915.140000001</v>
+        <v>23146412.949999999</v>
       </c>
       <c r="F37">
-        <v>23146412.949999999</v>
-      </c>
-      <c r="G37">
         <v>404</v>
       </c>
-      <c r="H37" t="s">
+      <c r="G37" t="s">
         <v>218</v>
       </c>
-      <c r="I37">
+      <c r="H37">
         <v>3793</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="1">
-        <v>36</v>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <v>12614.38</v>
       </c>
       <c r="C38">
-        <v>12614.38</v>
+        <v>0</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>77488.320000000007</v>
       </c>
       <c r="E38">
-        <v>77488.320000000007</v>
+        <v>90102.700000000012</v>
       </c>
       <c r="F38">
-        <v>90102.700000000012</v>
-      </c>
-      <c r="G38">
         <v>405</v>
       </c>
-      <c r="H38" t="s">
+      <c r="G38" t="s">
         <v>218</v>
       </c>
-      <c r="I38">
+      <c r="H38">
         <v>3793</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="1">
-        <v>37</v>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B39">
+        <v>2358257</v>
       </c>
       <c r="C39">
-        <v>2358257</v>
+        <v>0</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>14486436</v>
       </c>
       <c r="E39">
-        <v>14486436</v>
+        <v>16844693</v>
       </c>
       <c r="F39">
-        <v>16844693</v>
-      </c>
-      <c r="G39">
         <v>405</v>
       </c>
-      <c r="H39" t="s">
+      <c r="G39" t="s">
         <v>217</v>
       </c>
-      <c r="I39">
+      <c r="H39">
         <v>3791</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="1">
-        <v>38</v>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <v>1040132.45</v>
       </c>
       <c r="C40">
-        <v>1040132.45</v>
+        <v>0</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>6389385.0800000001</v>
       </c>
       <c r="E40">
-        <v>6389385.0800000001</v>
+        <v>7429517.5300000003</v>
       </c>
       <c r="F40">
-        <v>7429517.5300000003</v>
-      </c>
-      <c r="G40">
         <v>404</v>
       </c>
-      <c r="H40" t="s">
+      <c r="G40" t="s">
         <v>218</v>
       </c>
-      <c r="I40">
+      <c r="H40">
         <v>3795</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="1">
-        <v>39</v>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <v>417985.19</v>
       </c>
       <c r="C41">
-        <v>417985.19</v>
+        <v>0</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <v>2567623.2799999998</v>
       </c>
       <c r="E41">
-        <v>2567623.2799999998</v>
+        <v>2985608.47</v>
       </c>
       <c r="F41">
-        <v>2985608.47</v>
-      </c>
-      <c r="G41">
         <v>405</v>
       </c>
-      <c r="H41" t="s">
+      <c r="G41" t="s">
         <v>218</v>
       </c>
-      <c r="I41">
+      <c r="H41">
         <v>3795</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="1">
-        <v>40</v>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B42">
+        <v>638.30999999999995</v>
       </c>
       <c r="C42">
-        <v>638.30999999999995</v>
+        <v>0</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>3921.03</v>
       </c>
       <c r="E42">
-        <v>3921.03</v>
+        <v>4559.34</v>
       </c>
       <c r="F42">
-        <v>4559.34</v>
-      </c>
-      <c r="G42">
         <v>402</v>
       </c>
-      <c r="H42" t="s">
+      <c r="G42" t="s">
         <v>218</v>
       </c>
-      <c r="I42">
+      <c r="H42">
         <v>3796</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="1">
-        <v>41</v>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B43">
+        <v>18878.16</v>
       </c>
       <c r="C43">
-        <v>18878.16</v>
+        <v>0</v>
       </c>
       <c r="D43">
-        <v>0</v>
+        <v>115965.85</v>
       </c>
       <c r="E43">
-        <v>115965.85</v>
+        <v>134844.01</v>
       </c>
       <c r="F43">
-        <v>134844.01</v>
-      </c>
-      <c r="G43">
         <v>404</v>
       </c>
-      <c r="H43" t="s">
+      <c r="G43" t="s">
         <v>218</v>
       </c>
-      <c r="I43">
+      <c r="H43">
         <v>3796</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="1">
-        <v>42</v>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B44">
+        <v>16053.87</v>
       </c>
       <c r="C44">
-        <v>16053.87</v>
+        <v>0</v>
       </c>
       <c r="D44">
-        <v>0</v>
+        <v>98616.63</v>
       </c>
       <c r="E44">
-        <v>98616.63</v>
+        <v>114670.5</v>
       </c>
       <c r="F44">
-        <v>114670.5</v>
-      </c>
-      <c r="G44">
         <v>405</v>
       </c>
-      <c r="H44" t="s">
+      <c r="G44" t="s">
         <v>218</v>
       </c>
-      <c r="I44">
+      <c r="H44">
         <v>3796</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="1">
-        <v>43</v>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B45">
+        <v>2073062.48</v>
       </c>
       <c r="C45">
-        <v>2073062.48</v>
+        <v>0</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <v>12734526.48</v>
       </c>
       <c r="E45">
-        <v>12734526.48</v>
+        <v>14807588.960000001</v>
       </c>
       <c r="F45">
-        <v>14807588.960000001</v>
-      </c>
-      <c r="G45">
         <v>409</v>
       </c>
-      <c r="H45" t="s">
+      <c r="G45" t="s">
         <v>218</v>
       </c>
-      <c r="I45">
+      <c r="H45">
         <v>3796</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="1">
-        <v>44</v>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B46">
+        <v>18361.52</v>
       </c>
       <c r="C46">
-        <v>18361.52</v>
+        <v>0</v>
       </c>
       <c r="D46">
-        <v>0</v>
+        <v>112792.21</v>
       </c>
       <c r="E46">
-        <v>112792.21</v>
+        <v>131153.73000000001</v>
       </c>
       <c r="F46">
-        <v>131153.73000000001</v>
-      </c>
-      <c r="G46">
         <v>402</v>
       </c>
-      <c r="H46" t="s">
+      <c r="G46" t="s">
         <v>218</v>
       </c>
-      <c r="I46">
+      <c r="H46">
         <v>3797</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="1">
-        <v>45</v>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B47">
+        <v>2987789.88</v>
       </c>
       <c r="C47">
-        <v>2987789.88</v>
+        <v>0</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <v>18353566.390000001</v>
       </c>
       <c r="E47">
-        <v>18353566.390000001</v>
+        <v>21341356.27</v>
       </c>
       <c r="F47">
-        <v>21341356.27</v>
-      </c>
-      <c r="G47">
         <v>404</v>
       </c>
-      <c r="H47" t="s">
+      <c r="G47" t="s">
         <v>218</v>
       </c>
-      <c r="I47">
+      <c r="H47">
         <v>3797</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="1">
-        <v>46</v>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B48">
+        <v>2205484.6800000002</v>
       </c>
       <c r="C48">
-        <v>2205484.6800000002</v>
+        <v>0</v>
       </c>
       <c r="D48">
-        <v>0</v>
+        <v>13547977.32</v>
       </c>
       <c r="E48">
-        <v>13547977.32</v>
+        <v>15753462</v>
       </c>
       <c r="F48">
-        <v>15753462</v>
-      </c>
-      <c r="G48">
         <v>409</v>
       </c>
-      <c r="H48" t="s">
+      <c r="G48" t="s">
         <v>219</v>
       </c>
-      <c r="I48">
+      <c r="H48">
         <v>3805</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="1">
-        <v>47</v>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B49">
+        <v>282389.38</v>
       </c>
       <c r="C49">
-        <v>282389.38</v>
+        <v>0</v>
       </c>
       <c r="D49">
-        <v>0</v>
+        <v>1734677.62</v>
       </c>
       <c r="E49">
-        <v>1734677.62</v>
+        <v>2017067</v>
       </c>
       <c r="F49">
-        <v>2017067</v>
-      </c>
-      <c r="G49">
         <v>405</v>
       </c>
-      <c r="H49" t="s">
+      <c r="G49" t="s">
         <v>220</v>
       </c>
-      <c r="I49">
+      <c r="H49">
         <v>3812</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="1">
-        <v>48</v>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B50">
+        <v>2767259.32</v>
       </c>
       <c r="C50">
-        <v>2767259.32</v>
+        <v>0</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <v>16998878.68</v>
       </c>
       <c r="E50">
-        <v>16998878.68</v>
+        <v>19766138</v>
       </c>
       <c r="F50">
-        <v>19766138</v>
-      </c>
-      <c r="G50">
         <v>405</v>
       </c>
-      <c r="H50" t="s">
+      <c r="G50" t="s">
         <v>221</v>
       </c>
-      <c r="I50">
+      <c r="H50">
         <v>3813</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="1">
-        <v>49</v>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B51">
+        <v>1580555.99</v>
       </c>
       <c r="C51">
-        <v>1580555.99</v>
+        <v>0</v>
       </c>
       <c r="D51">
-        <v>0</v>
+        <v>10577567.01</v>
       </c>
       <c r="E51">
-        <v>10577567.01</v>
+        <v>12158123</v>
       </c>
       <c r="F51">
-        <v>12158123</v>
-      </c>
-      <c r="G51">
         <v>404</v>
       </c>
-      <c r="H51" t="s">
+      <c r="G51" t="s">
         <v>221</v>
       </c>
-      <c r="I51">
+      <c r="H51">
         <v>3816</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="1">
-        <v>50</v>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B52">
+        <v>309991.96000000002</v>
       </c>
       <c r="C52">
-        <v>309991.96000000002</v>
+        <v>0</v>
       </c>
       <c r="D52">
-        <v>0</v>
+        <v>2056100.04</v>
       </c>
       <c r="E52">
-        <v>2056100.04</v>
+        <v>2366092</v>
       </c>
       <c r="F52">
-        <v>2366092</v>
-      </c>
-      <c r="G52">
         <v>404</v>
       </c>
-      <c r="H52" t="s">
+      <c r="G52" t="s">
         <v>222</v>
       </c>
-      <c r="I52">
+      <c r="H52">
         <v>3824</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="1">
-        <v>51</v>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B53">
+        <v>962126</v>
       </c>
       <c r="C53">
-        <v>962126</v>
+        <v>0</v>
       </c>
       <c r="D53">
-        <v>0</v>
+        <v>6438840</v>
       </c>
       <c r="E53">
-        <v>6438840</v>
+        <v>7400966</v>
       </c>
       <c r="F53">
-        <v>7400966</v>
-      </c>
-      <c r="G53">
         <v>405</v>
       </c>
-      <c r="H53" t="s">
+      <c r="G53" t="s">
         <v>223</v>
       </c>
-      <c r="I53">
+      <c r="H53">
         <v>3825</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="1">
-        <v>52</v>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B54">
+        <v>3498228.58</v>
       </c>
       <c r="C54">
-        <v>3498228.58</v>
+        <v>0</v>
       </c>
       <c r="D54">
-        <v>0</v>
+        <v>21489118.420000002</v>
       </c>
       <c r="E54">
-        <v>21489118.420000002</v>
+        <v>24987347</v>
       </c>
       <c r="F54">
-        <v>24987347</v>
-      </c>
-      <c r="G54">
         <v>407</v>
       </c>
-      <c r="H54" t="s">
+      <c r="G54" t="s">
         <v>224</v>
       </c>
-      <c r="I54">
+      <c r="H54">
         <v>3826</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="1">
-        <v>53</v>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B55">
+        <v>1093173.6200000001</v>
       </c>
       <c r="C55">
-        <v>1093173.6200000001</v>
+        <v>0</v>
       </c>
       <c r="D55">
-        <v>0</v>
+        <v>6715209.3799999999</v>
       </c>
       <c r="E55">
-        <v>6715209.3799999999</v>
+        <v>7808383</v>
       </c>
       <c r="F55">
-        <v>7808383</v>
-      </c>
-      <c r="G55">
         <v>405</v>
       </c>
-      <c r="H55" t="s">
+      <c r="G55" t="s">
         <v>225</v>
       </c>
-      <c r="I55">
+      <c r="H55">
         <v>3828</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="1">
-        <v>54</v>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B56">
+        <v>3116865.5</v>
       </c>
       <c r="C56">
-        <v>3116865.5</v>
+        <v>0</v>
       </c>
       <c r="D56">
-        <v>0</v>
+        <v>19146459.5</v>
       </c>
       <c r="E56">
-        <v>19146459.5</v>
+        <v>22263325</v>
       </c>
       <c r="F56">
-        <v>22263325</v>
-      </c>
-      <c r="G56">
         <v>404</v>
       </c>
-      <c r="H56" t="s">
+      <c r="G56" t="s">
         <v>226</v>
       </c>
-      <c r="I56">
+      <c r="H56">
         <v>3834</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="1">
-        <v>55</v>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B57">
+        <v>695132.1</v>
       </c>
       <c r="C57">
-        <v>695132.1</v>
+        <v>0</v>
       </c>
       <c r="D57">
-        <v>0</v>
+        <v>4652037.9000000004</v>
       </c>
       <c r="E57">
-        <v>4652037.9000000004</v>
+        <v>5347170</v>
       </c>
       <c r="F57">
-        <v>5347170</v>
-      </c>
-      <c r="G57">
         <v>405</v>
       </c>
-      <c r="H57" t="s">
+      <c r="G57" t="s">
         <v>226</v>
       </c>
-      <c r="I57">
+      <c r="H57">
         <v>3831</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="1">
-        <v>56</v>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B58">
+        <v>912258.48</v>
       </c>
       <c r="C58">
-        <v>912258.48</v>
+        <v>0</v>
       </c>
       <c r="D58">
-        <v>0</v>
+        <v>5603873.5199999996</v>
       </c>
       <c r="E58">
-        <v>5603873.5199999996</v>
+        <v>6516132</v>
       </c>
       <c r="F58">
-        <v>6516132</v>
-      </c>
-      <c r="G58">
         <v>405</v>
       </c>
-      <c r="H58" t="s">
+      <c r="G58" t="s">
         <v>226</v>
       </c>
-      <c r="I58">
+      <c r="H58">
         <v>3835</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="1">
-        <v>57</v>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B59">
+        <v>13642.2</v>
       </c>
       <c r="C59">
-        <v>13642.2</v>
+        <v>0</v>
       </c>
       <c r="D59">
-        <v>0</v>
+        <v>83802.05</v>
       </c>
       <c r="E59">
-        <v>83802.05</v>
+        <v>97444.25</v>
       </c>
       <c r="F59">
-        <v>97444.25</v>
-      </c>
-      <c r="G59">
         <v>402</v>
       </c>
-      <c r="H59" t="s">
+      <c r="G59" t="s">
         <v>226</v>
       </c>
-      <c r="I59">
+      <c r="H59">
         <v>3838</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="1">
-        <v>58</v>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B60">
+        <v>4958392.9800000004</v>
       </c>
       <c r="C60">
-        <v>4958392.9800000004</v>
+        <v>0</v>
       </c>
       <c r="D60">
-        <v>0</v>
+        <v>30458699.760000002</v>
       </c>
       <c r="E60">
-        <v>30458699.760000002</v>
+        <v>35417092.740000002</v>
       </c>
       <c r="F60">
-        <v>35417092.740000002</v>
-      </c>
-      <c r="G60">
         <v>404</v>
       </c>
-      <c r="H60" t="s">
+      <c r="G60" t="s">
         <v>226</v>
       </c>
-      <c r="I60">
+      <c r="H60">
         <v>3838</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="1">
-        <v>59</v>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B61">
+        <v>2110666.1800000002</v>
       </c>
       <c r="C61">
-        <v>2110666.1800000002</v>
+        <v>0</v>
       </c>
       <c r="D61">
-        <v>0</v>
+        <v>12965520.82</v>
       </c>
       <c r="E61">
-        <v>12965520.82</v>
+        <v>15076187</v>
       </c>
       <c r="F61">
-        <v>15076187</v>
-      </c>
-      <c r="G61">
         <v>404</v>
       </c>
-      <c r="H61" t="s">
+      <c r="G61" t="s">
         <v>226</v>
       </c>
-      <c r="I61">
+      <c r="H61">
         <v>3832</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="1">
-        <v>60</v>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B62">
+        <v>4781808.08</v>
       </c>
       <c r="C62">
-        <v>4781808.08</v>
+        <v>0</v>
       </c>
       <c r="D62">
-        <v>0</v>
+        <v>29373963.920000002</v>
       </c>
       <c r="E62">
-        <v>29373963.920000002</v>
+        <v>34155772</v>
       </c>
       <c r="F62">
-        <v>34155772</v>
-      </c>
-      <c r="G62">
         <v>406</v>
       </c>
-      <c r="H62" t="s">
+      <c r="G62" t="s">
         <v>226</v>
       </c>
-      <c r="I62">
+      <c r="H62">
         <v>3836</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="1">
-        <v>61</v>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B63">
+        <v>2111180.4</v>
       </c>
       <c r="C63">
-        <v>2111180.4</v>
+        <v>0</v>
       </c>
       <c r="D63">
-        <v>0</v>
+        <v>12968679.6</v>
       </c>
       <c r="E63">
-        <v>12968679.6</v>
+        <v>15079860</v>
       </c>
       <c r="F63">
-        <v>15079860</v>
-      </c>
-      <c r="G63">
         <v>406</v>
       </c>
-      <c r="H63" t="s">
+      <c r="G63" t="s">
         <v>226</v>
       </c>
-      <c r="I63">
+      <c r="H63">
         <v>3833</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="1">
-        <v>62</v>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B64">
+        <v>651367.74</v>
       </c>
       <c r="C64">
-        <v>651367.74</v>
+        <v>0</v>
       </c>
       <c r="D64">
-        <v>0</v>
+        <v>4001258.99</v>
       </c>
       <c r="E64">
-        <v>4001258.99</v>
+        <v>4652626.7300000004</v>
       </c>
       <c r="F64">
-        <v>4652626.7300000004</v>
-      </c>
-      <c r="G64">
         <v>404</v>
       </c>
-      <c r="H64" t="s">
+      <c r="G64" t="s">
         <v>226</v>
       </c>
-      <c r="I64">
+      <c r="H64">
         <v>3839</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A65" s="1">
-        <v>63</v>
+    <row r="65" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B65">
+        <v>416916.82</v>
       </c>
       <c r="C65">
-        <v>416916.82</v>
+        <v>0</v>
       </c>
       <c r="D65">
-        <v>0</v>
+        <v>2561060.4500000002</v>
       </c>
       <c r="E65">
-        <v>2561060.4500000002</v>
+        <v>2977977.27</v>
       </c>
       <c r="F65">
-        <v>2977977.27</v>
-      </c>
-      <c r="G65">
         <v>405</v>
       </c>
-      <c r="H65" t="s">
+      <c r="G65" t="s">
         <v>226</v>
       </c>
-      <c r="I65">
+      <c r="H65">
         <v>3839</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A66" s="1">
-        <v>64</v>
+    <row r="66" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B66">
+        <v>3754312.24</v>
       </c>
       <c r="C66">
-        <v>3754312.24</v>
+        <v>0</v>
       </c>
       <c r="D66">
-        <v>0</v>
+        <v>23062203.760000002</v>
       </c>
       <c r="E66">
-        <v>23062203.760000002</v>
+        <v>26816516</v>
       </c>
       <c r="F66">
-        <v>26816516</v>
-      </c>
-      <c r="G66">
         <v>404</v>
       </c>
-      <c r="H66" t="s">
+      <c r="G66" t="s">
         <v>227</v>
       </c>
-      <c r="I66">
+      <c r="H66">
         <v>3847</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A67" s="1">
-        <v>65</v>
+    <row r="67" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B67">
+        <v>1675667.7</v>
       </c>
       <c r="C67">
-        <v>1675667.7</v>
+        <v>0</v>
       </c>
       <c r="D67">
-        <v>0</v>
+        <v>10293387.300000001</v>
       </c>
       <c r="E67">
-        <v>10293387.300000001</v>
+        <v>11969055</v>
       </c>
       <c r="F67">
-        <v>11969055</v>
-      </c>
-      <c r="G67">
         <v>405</v>
       </c>
-      <c r="H67" t="s">
+      <c r="G67" t="s">
         <v>228</v>
       </c>
-      <c r="I67">
+      <c r="H67">
         <v>3849</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A68" s="1">
-        <v>66</v>
+    <row r="68" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B68">
+        <v>298004.2</v>
       </c>
       <c r="C68">
-        <v>298004.2</v>
+        <v>0</v>
       </c>
       <c r="D68">
-        <v>0</v>
+        <v>1994335.8</v>
       </c>
       <c r="E68">
-        <v>1994335.8</v>
+        <v>2292340</v>
       </c>
       <c r="F68">
-        <v>2292340</v>
-      </c>
-      <c r="G68">
         <v>404</v>
       </c>
-      <c r="H68" t="s">
+      <c r="G68" t="s">
         <v>229</v>
       </c>
-      <c r="I68">
+      <c r="H68">
         <v>3858</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A69" s="1">
-        <v>67</v>
+    <row r="69" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B69">
+        <v>487051.18</v>
       </c>
       <c r="C69">
-        <v>487051.18</v>
+        <v>0</v>
       </c>
       <c r="D69">
-        <v>0</v>
+        <v>2991885.82</v>
       </c>
       <c r="E69">
-        <v>2991885.82</v>
+        <v>3478937</v>
       </c>
       <c r="F69">
-        <v>3478937</v>
-      </c>
-      <c r="G69">
         <v>409</v>
       </c>
-      <c r="H69" t="s">
+      <c r="G69" t="s">
         <v>230</v>
       </c>
-      <c r="I69">
+      <c r="H69">
         <v>3859</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A70" s="1">
-        <v>68</v>
+    <row r="70" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B70">
+        <v>7310.76</v>
       </c>
       <c r="C70">
-        <v>7310.76</v>
+        <v>0</v>
       </c>
       <c r="D70">
-        <v>0</v>
+        <v>44908.93</v>
       </c>
       <c r="E70">
-        <v>44908.93</v>
+        <v>52219.69</v>
       </c>
       <c r="F70">
-        <v>52219.69</v>
-      </c>
-      <c r="G70">
         <v>402</v>
       </c>
-      <c r="H70" t="s">
+      <c r="G70" t="s">
         <v>231</v>
       </c>
-      <c r="I70">
+      <c r="H70">
         <v>3867</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A71" s="1">
-        <v>69</v>
+    <row r="71" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B71">
+        <v>2212144.9700000002</v>
       </c>
       <c r="C71">
-        <v>2212144.9700000002</v>
+        <v>0</v>
       </c>
       <c r="D71">
-        <v>0</v>
+        <v>13588890.550000001</v>
       </c>
       <c r="E71">
-        <v>13588890.550000001</v>
+        <v>15801035.52</v>
       </c>
       <c r="F71">
-        <v>15801035.52</v>
-      </c>
-      <c r="G71">
         <v>404</v>
       </c>
-      <c r="H71" t="s">
+      <c r="G71" t="s">
         <v>231</v>
       </c>
-      <c r="I71">
+      <c r="H71">
         <v>3867</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A72" s="1">
-        <v>70</v>
+    <row r="72" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B72">
+        <v>992707.49</v>
       </c>
       <c r="C72">
-        <v>992707.49</v>
+        <v>0</v>
       </c>
       <c r="D72">
-        <v>0</v>
+        <v>6098060.2999999998</v>
       </c>
       <c r="E72">
-        <v>6098060.2999999998</v>
+        <v>7090767.79</v>
       </c>
       <c r="F72">
-        <v>7090767.79</v>
-      </c>
-      <c r="G72">
         <v>405</v>
       </c>
-      <c r="H72" t="s">
+      <c r="G72" t="s">
         <v>231</v>
       </c>
-      <c r="I72">
+      <c r="H72">
         <v>3867</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A73" s="1">
-        <v>71</v>
+    <row r="73" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B73">
+        <v>1423590</v>
       </c>
       <c r="C73">
-        <v>1423590</v>
+        <v>0</v>
       </c>
       <c r="D73">
-        <v>0</v>
+        <v>8744910</v>
       </c>
       <c r="E73">
-        <v>8744910</v>
+        <v>10168500</v>
       </c>
       <c r="F73">
-        <v>10168500</v>
-      </c>
-      <c r="G73">
         <v>404</v>
       </c>
-      <c r="H73" t="s">
+      <c r="G73" t="s">
         <v>232</v>
       </c>
-      <c r="I73">
+      <c r="H73">
         <v>3872</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A74" s="1">
-        <v>72</v>
+    <row r="74" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B74">
+        <v>2174449.9</v>
       </c>
       <c r="C74">
-        <v>2174449.9</v>
+        <v>0</v>
       </c>
       <c r="D74">
-        <v>0</v>
+        <v>13357335.1</v>
       </c>
       <c r="E74">
-        <v>13357335.1</v>
+        <v>15531785</v>
       </c>
       <c r="F74">
-        <v>15531785</v>
-      </c>
-      <c r="G74">
         <v>409</v>
       </c>
-      <c r="H74" t="s">
+      <c r="G74" t="s">
         <v>232</v>
       </c>
-      <c r="I74">
+      <c r="H74">
         <v>3873</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A75" s="1">
-        <v>73</v>
+    <row r="75" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B75">
+        <v>261.86</v>
       </c>
       <c r="C75">
-        <v>261.86</v>
+        <v>0</v>
       </c>
       <c r="D75">
-        <v>0</v>
+        <v>1608.59</v>
       </c>
       <c r="E75">
-        <v>1608.59</v>
+        <v>1870.45</v>
       </c>
       <c r="F75">
-        <v>1870.45</v>
-      </c>
-      <c r="G75">
         <v>402</v>
       </c>
-      <c r="H75" t="s">
+      <c r="G75" t="s">
         <v>232</v>
       </c>
-      <c r="I75">
+      <c r="H75">
         <v>3872</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A76" s="1">
-        <v>74</v>
+    <row r="76" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B76">
+        <v>7744.69</v>
       </c>
       <c r="C76">
-        <v>7744.69</v>
+        <v>0</v>
       </c>
       <c r="D76">
-        <v>0</v>
+        <v>47574.51</v>
       </c>
       <c r="E76">
-        <v>47574.51</v>
+        <v>55319.199999999997</v>
       </c>
       <c r="F76">
-        <v>55319.199999999997</v>
-      </c>
-      <c r="G76">
         <v>404</v>
       </c>
-      <c r="H76" t="s">
+      <c r="G76" t="s">
         <v>232</v>
       </c>
-      <c r="I76">
+      <c r="H76">
         <v>3872</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A77" s="1">
-        <v>75</v>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B77">
+        <v>2439531.13</v>
       </c>
       <c r="C77">
-        <v>2439531.13</v>
+        <v>0</v>
       </c>
       <c r="D77">
-        <v>0</v>
+        <v>14985691.24</v>
       </c>
       <c r="E77">
-        <v>14985691.24</v>
+        <v>17425222.370000001</v>
       </c>
       <c r="F77">
-        <v>17425222.370000001</v>
-      </c>
-      <c r="G77">
         <v>405</v>
       </c>
-      <c r="H77" t="s">
+      <c r="G77" t="s">
         <v>232</v>
       </c>
-      <c r="I77">
+      <c r="H77">
         <v>3872</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A78" s="1">
-        <v>76</v>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B78">
+        <v>1738788.1</v>
       </c>
       <c r="C78">
-        <v>1738788.1</v>
+        <v>0</v>
       </c>
       <c r="D78">
-        <v>0</v>
+        <v>10681126.890000001</v>
       </c>
       <c r="E78">
-        <v>10681126.890000001</v>
+        <v>12419914.99</v>
       </c>
       <c r="F78">
-        <v>12419914.99</v>
-      </c>
-      <c r="G78">
         <v>409</v>
       </c>
-      <c r="H78" t="s">
+      <c r="G78" t="s">
         <v>232</v>
       </c>
-      <c r="I78">
+      <c r="H78">
         <v>3872</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A79" s="1">
-        <v>77</v>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B79">
+        <v>12552.4</v>
       </c>
       <c r="C79">
-        <v>12552.4</v>
+        <v>0</v>
       </c>
       <c r="D79">
-        <v>0</v>
+        <v>77107.600000000006</v>
       </c>
       <c r="E79">
-        <v>77107.600000000006</v>
+        <v>89660</v>
       </c>
       <c r="F79">
-        <v>89660</v>
-      </c>
-      <c r="G79">
         <v>403</v>
       </c>
-      <c r="H79" t="s">
+      <c r="G79" t="s">
         <v>232</v>
       </c>
-      <c r="I79">
+      <c r="H79">
         <v>3871</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A80" s="1">
-        <v>78</v>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B80">
+        <v>14506.8</v>
       </c>
       <c r="C80">
-        <v>14506.8</v>
+        <v>0</v>
       </c>
       <c r="D80">
-        <v>0</v>
+        <v>89113.2</v>
       </c>
       <c r="E80">
-        <v>89113.2</v>
+        <v>103620</v>
       </c>
       <c r="F80">
-        <v>103620</v>
-      </c>
-      <c r="G80">
         <v>407</v>
       </c>
-      <c r="H80" t="s">
+      <c r="G80" t="s">
         <v>232</v>
       </c>
-      <c r="I80">
+      <c r="H80">
         <v>3871</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A81" s="1">
-        <v>79</v>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B81">
+        <v>2056634.44</v>
       </c>
       <c r="C81">
-        <v>2056634.44</v>
+        <v>0</v>
       </c>
       <c r="D81">
-        <v>0</v>
+        <v>12633611.560000001</v>
       </c>
       <c r="E81">
-        <v>12633611.560000001</v>
+        <v>14690246</v>
       </c>
       <c r="F81">
-        <v>14690246</v>
-      </c>
-      <c r="G81">
         <v>408</v>
       </c>
-      <c r="H81" t="s">
+      <c r="G81" t="s">
         <v>232</v>
       </c>
-      <c r="I81">
+      <c r="H81">
         <v>3871</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A82" s="1">
-        <v>80</v>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B82">
+        <v>437340.15</v>
       </c>
       <c r="C82">
-        <v>437340.15</v>
+        <v>0</v>
       </c>
       <c r="D82">
-        <v>0</v>
+        <v>2926814.85</v>
       </c>
       <c r="E82">
-        <v>2926814.85</v>
+        <v>3364155</v>
       </c>
       <c r="F82">
-        <v>3364155</v>
-      </c>
-      <c r="G82">
         <v>405</v>
       </c>
-      <c r="H82" t="s">
+      <c r="G82" t="s">
         <v>233</v>
       </c>
-      <c r="I82">
+      <c r="H82">
         <v>3885</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A83" s="1">
-        <v>81</v>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B83">
+        <v>845322.83</v>
       </c>
       <c r="C83">
-        <v>845322.83</v>
+        <v>0</v>
       </c>
       <c r="D83">
-        <v>0</v>
+        <v>5192697.3600000003</v>
       </c>
       <c r="E83">
-        <v>5192697.3600000003</v>
+        <v>6038020.1900000004</v>
       </c>
       <c r="F83">
-        <v>6038020.1900000004</v>
-      </c>
-      <c r="G83">
         <v>404</v>
       </c>
-      <c r="H83" t="s">
+      <c r="G83" t="s">
         <v>233</v>
       </c>
-      <c r="I83">
+      <c r="H83">
         <v>3886</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A84" s="1">
-        <v>82</v>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B84">
+        <v>49031.19</v>
       </c>
       <c r="C84">
-        <v>49031.19</v>
+        <v>0</v>
       </c>
       <c r="D84">
-        <v>0</v>
+        <v>301191.62</v>
       </c>
       <c r="E84">
-        <v>301191.62</v>
+        <v>350222.81</v>
       </c>
       <c r="F84">
-        <v>350222.81</v>
-      </c>
-      <c r="G84">
         <v>405</v>
       </c>
-      <c r="H84" t="s">
+      <c r="G84" t="s">
         <v>233</v>
       </c>
-      <c r="I84">
+      <c r="H84">
         <v>3886</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A85" s="1">
-        <v>83</v>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B85">
+        <v>500414.6</v>
       </c>
       <c r="C85">
-        <v>500414.6</v>
+        <v>0</v>
       </c>
       <c r="D85">
-        <v>0</v>
+        <v>3073975.4</v>
       </c>
       <c r="E85">
-        <v>3073975.4</v>
+        <v>3574390</v>
       </c>
       <c r="F85">
-        <v>3574390</v>
-      </c>
-      <c r="G85">
         <v>405</v>
       </c>
-      <c r="H85" t="s">
+      <c r="G85" t="s">
         <v>233</v>
       </c>
-      <c r="I85">
+      <c r="H85">
         <v>3887</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A86" s="1">
-        <v>84</v>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B86">
+        <v>2088646.84</v>
       </c>
       <c r="C86">
-        <v>2088646.84</v>
+        <v>0</v>
       </c>
       <c r="D86">
-        <v>0</v>
+        <v>12830259.16</v>
       </c>
       <c r="E86">
-        <v>12830259.16</v>
+        <v>14918906</v>
       </c>
       <c r="F86">
-        <v>14918906</v>
-      </c>
-      <c r="G86">
         <v>406</v>
       </c>
-      <c r="H86" t="s">
+      <c r="G86" t="s">
         <v>234</v>
       </c>
-      <c r="I86">
+      <c r="H86">
         <v>3911</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A87" s="1">
-        <v>85</v>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B87">
+        <v>533385.87</v>
       </c>
       <c r="C87">
-        <v>533385.87</v>
+        <v>0</v>
       </c>
       <c r="D87">
-        <v>0</v>
+        <v>3276513.16</v>
       </c>
       <c r="E87">
-        <v>3276513.16</v>
+        <v>3809899.03</v>
       </c>
       <c r="F87">
-        <v>3809899.03</v>
-      </c>
-      <c r="G87">
         <v>404</v>
       </c>
-      <c r="H87" t="s">
+      <c r="G87" t="s">
         <v>234</v>
       </c>
-      <c r="I87">
+      <c r="H87">
         <v>3912</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A88" s="1">
-        <v>86</v>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B88">
+        <v>760457.03</v>
       </c>
       <c r="C88">
-        <v>760457.03</v>
+        <v>0</v>
       </c>
       <c r="D88">
-        <v>0</v>
+        <v>4671378.84</v>
       </c>
       <c r="E88">
-        <v>4671378.84</v>
+        <v>5431835.8700000001</v>
       </c>
       <c r="F88">
-        <v>5431835.8700000001</v>
-      </c>
-      <c r="G88">
         <v>405</v>
       </c>
-      <c r="H88" t="s">
+      <c r="G88" t="s">
         <v>234</v>
       </c>
-      <c r="I88">
+      <c r="H88">
         <v>3912</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A89" s="1">
-        <v>87</v>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B89">
+        <v>819426.03</v>
       </c>
       <c r="C89">
-        <v>819426.03</v>
+        <v>0</v>
       </c>
       <c r="D89">
-        <v>0</v>
+        <v>5033617.07</v>
       </c>
       <c r="E89">
-        <v>5033617.07</v>
+        <v>5853043.1000000006</v>
       </c>
       <c r="F89">
-        <v>5853043.1000000006</v>
-      </c>
-      <c r="G89">
         <v>404</v>
       </c>
-      <c r="H89" t="s">
+      <c r="G89" t="s">
         <v>235</v>
       </c>
-      <c r="I89">
+      <c r="H89">
         <v>3926</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A90" s="1">
-        <v>88</v>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B90">
+        <v>782941.73</v>
       </c>
       <c r="C90">
-        <v>782941.73</v>
+        <v>0</v>
       </c>
       <c r="D90">
-        <v>0</v>
+        <v>4809499.17</v>
       </c>
       <c r="E90">
-        <v>4809499.17</v>
+        <v>5592440.9000000004</v>
       </c>
       <c r="F90">
-        <v>5592440.9000000004</v>
-      </c>
-      <c r="G90">
         <v>405</v>
       </c>
-      <c r="H90" t="s">
+      <c r="G90" t="s">
         <v>235</v>
       </c>
-      <c r="I90">
+      <c r="H90">
         <v>3926</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A91" s="1">
-        <v>89</v>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B91">
+        <v>1268086.96</v>
       </c>
       <c r="C91">
-        <v>1268086.96</v>
+        <v>0</v>
       </c>
       <c r="D91">
-        <v>0</v>
+        <v>7789677.04</v>
       </c>
       <c r="E91">
-        <v>7789677.04</v>
+        <v>9057764</v>
       </c>
       <c r="F91">
-        <v>9057764</v>
-      </c>
-      <c r="G91">
         <v>405</v>
       </c>
-      <c r="H91" t="s">
+      <c r="G91" t="s">
         <v>235</v>
       </c>
-      <c r="I91">
+      <c r="H91">
         <v>3921</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A92" s="1">
-        <v>90</v>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B92">
+        <v>270136.46000000002</v>
       </c>
       <c r="C92">
-        <v>270136.46000000002</v>
+        <v>0</v>
       </c>
       <c r="D92">
-        <v>0</v>
+        <v>1659409.69</v>
       </c>
       <c r="E92">
-        <v>1659409.69</v>
+        <v>1929546.15</v>
       </c>
       <c r="F92">
-        <v>1929546.15</v>
-      </c>
-      <c r="G92">
         <v>404</v>
       </c>
-      <c r="H92" t="s">
+      <c r="G92" t="s">
         <v>235</v>
       </c>
-      <c r="I92">
+      <c r="H92">
         <v>3922</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A93" s="1">
-        <v>91</v>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B93">
+        <v>277546.34000000003</v>
       </c>
       <c r="C93">
-        <v>277546.34000000003</v>
+        <v>0</v>
       </c>
       <c r="D93">
-        <v>0</v>
+        <v>1704927.51</v>
       </c>
       <c r="E93">
-        <v>1704927.51</v>
+        <v>1982473.85</v>
       </c>
       <c r="F93">
-        <v>1982473.85</v>
-      </c>
-      <c r="G93">
         <v>405</v>
       </c>
-      <c r="H93" t="s">
+      <c r="G93" t="s">
         <v>235</v>
       </c>
-      <c r="I93">
+      <c r="H93">
         <v>3922</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A94" s="1">
-        <v>92</v>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B94">
+        <v>2123862</v>
       </c>
       <c r="C94">
-        <v>2123862</v>
+        <v>0</v>
       </c>
       <c r="D94">
-        <v>0</v>
+        <v>13046585.279999999</v>
       </c>
       <c r="E94">
-        <v>13046585.279999999</v>
+        <v>15170447.279999999</v>
       </c>
       <c r="F94">
-        <v>15170447.279999999</v>
-      </c>
-      <c r="G94">
         <v>405</v>
       </c>
-      <c r="H94" t="s">
+      <c r="G94" t="s">
         <v>235</v>
       </c>
-      <c r="I94">
+      <c r="H94">
         <v>3925</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A95" s="1">
-        <v>93</v>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B95">
+        <v>221348.12</v>
       </c>
       <c r="C95">
-        <v>221348.12</v>
+        <v>0</v>
       </c>
       <c r="D95">
-        <v>0</v>
+        <v>1359709.88</v>
       </c>
       <c r="E95">
-        <v>1359709.88</v>
+        <v>1581058</v>
       </c>
       <c r="F95">
-        <v>1581058</v>
-      </c>
-      <c r="G95">
         <v>402</v>
       </c>
-      <c r="H95" t="s">
+      <c r="G95" t="s">
         <v>235</v>
       </c>
-      <c r="I95">
+      <c r="H95">
         <v>3927</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A96" s="1">
-        <v>94</v>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B96">
+        <v>1596431.34</v>
       </c>
       <c r="C96">
-        <v>1596431.34</v>
+        <v>0</v>
       </c>
       <c r="D96">
-        <v>0</v>
+        <v>9806649.6600000001</v>
       </c>
       <c r="E96">
-        <v>9806649.6600000001</v>
+        <v>11403081</v>
       </c>
       <c r="F96">
-        <v>11403081</v>
-      </c>
-      <c r="G96">
         <v>404</v>
       </c>
-      <c r="H96" t="s">
+      <c r="G96" t="s">
         <v>235</v>
       </c>
-      <c r="I96">
+      <c r="H96">
         <v>3927</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A97" s="1">
-        <v>95</v>
+    <row r="97" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B97">
+        <v>14676.2</v>
       </c>
       <c r="C97">
-        <v>14676.2</v>
+        <v>0</v>
       </c>
       <c r="D97">
-        <v>0</v>
+        <v>90153.8</v>
       </c>
       <c r="E97">
-        <v>90153.8</v>
+        <v>104830</v>
       </c>
       <c r="F97">
-        <v>104830</v>
-      </c>
-      <c r="G97">
         <v>402</v>
       </c>
-      <c r="H97" t="s">
+      <c r="G97" t="s">
         <v>235</v>
       </c>
-      <c r="I97">
+      <c r="H97">
         <v>3923</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A98" s="1">
-        <v>96</v>
+    <row r="98" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B98">
+        <v>3562630.56</v>
       </c>
       <c r="C98">
-        <v>3562630.56</v>
+        <v>0</v>
       </c>
       <c r="D98">
-        <v>0</v>
+        <v>21884724.440000001</v>
       </c>
       <c r="E98">
-        <v>21884724.440000001</v>
+        <v>25447355</v>
       </c>
       <c r="F98">
-        <v>25447355</v>
-      </c>
-      <c r="G98">
         <v>404</v>
       </c>
-      <c r="H98" t="s">
+      <c r="G98" t="s">
         <v>235</v>
       </c>
-      <c r="I98">
+      <c r="H98">
         <v>3923</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A99" s="1">
-        <v>97</v>
+    <row r="99" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B99">
+        <v>1426521</v>
       </c>
       <c r="C99">
-        <v>1426521</v>
+        <v>0</v>
       </c>
       <c r="D99">
-        <v>0</v>
+        <v>8763629</v>
       </c>
       <c r="E99">
-        <v>8763629</v>
+        <v>10190150</v>
       </c>
       <c r="F99">
-        <v>10190150</v>
-      </c>
-      <c r="G99">
         <v>406</v>
       </c>
-      <c r="H99" t="s">
+      <c r="G99" t="s">
         <v>235</v>
       </c>
-      <c r="I99">
+      <c r="H99">
         <v>3920</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A100" s="1">
-        <v>98</v>
+    <row r="100" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B100">
+        <v>2101471.96</v>
       </c>
       <c r="C100">
-        <v>2101471.96</v>
+        <v>0</v>
       </c>
       <c r="D100">
-        <v>0</v>
+        <v>12909042.039999999</v>
       </c>
       <c r="E100">
-        <v>12909042.039999999</v>
+        <v>15010514</v>
       </c>
       <c r="F100">
-        <v>15010514</v>
-      </c>
-      <c r="G100">
         <v>405</v>
       </c>
-      <c r="H100" t="s">
+      <c r="G100" t="s">
         <v>235</v>
       </c>
-      <c r="I100">
+      <c r="H100">
         <v>3924</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A101" s="1">
-        <v>99</v>
+    <row r="101" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B101">
+        <v>920500</v>
       </c>
       <c r="C101">
-        <v>920500</v>
+        <v>0</v>
       </c>
       <c r="D101">
-        <v>0</v>
+        <v>5654500</v>
       </c>
       <c r="E101">
-        <v>5654500</v>
+        <v>6575000</v>
       </c>
       <c r="F101">
-        <v>6575000</v>
-      </c>
-      <c r="G101">
         <v>405</v>
       </c>
-      <c r="H101" t="s">
+      <c r="G101" t="s">
         <v>235</v>
       </c>
-      <c r="I101">
+      <c r="H101">
         <v>3928</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A102" s="1">
-        <v>100</v>
+    <row r="102" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B102">
+        <v>756830</v>
       </c>
       <c r="C102">
-        <v>756830</v>
+        <v>0</v>
       </c>
       <c r="D102">
-        <v>0</v>
+        <v>5673258</v>
       </c>
       <c r="E102">
-        <v>5673258</v>
+        <v>6430088</v>
       </c>
       <c r="F102">
-        <v>6430088</v>
-      </c>
-      <c r="G102">
         <v>404</v>
       </c>
-      <c r="H102" t="s">
+      <c r="G102" t="s">
         <v>236</v>
       </c>
-      <c r="I102">
+      <c r="H102">
         <v>3930</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A103" s="1">
-        <v>101</v>
+    <row r="103" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B103">
+        <v>1176653.6599999999</v>
       </c>
       <c r="C103">
-        <v>1176653.6599999999</v>
+        <v>0</v>
       </c>
       <c r="D103">
-        <v>0</v>
+        <v>7228015.3399999999</v>
       </c>
       <c r="E103">
-        <v>7228015.3399999999</v>
+        <v>8404669</v>
       </c>
       <c r="F103">
-        <v>8404669</v>
-      </c>
-      <c r="G103">
         <v>408</v>
       </c>
-      <c r="H103" t="s">
+      <c r="G103" t="s">
         <v>237</v>
       </c>
-      <c r="I103">
+      <c r="H103">
         <v>3939</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A104" s="1">
-        <v>102</v>
+    <row r="104" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B104">
+        <v>230014.68</v>
       </c>
       <c r="C104">
-        <v>230014.68</v>
+        <v>0</v>
       </c>
       <c r="D104">
-        <v>0</v>
+        <v>1412947.32</v>
       </c>
       <c r="E104">
-        <v>1412947.32</v>
+        <v>1642962</v>
       </c>
       <c r="F104">
-        <v>1642962</v>
-      </c>
-      <c r="G104">
         <v>404</v>
       </c>
-      <c r="H104" t="s">
+      <c r="G104" t="s">
         <v>238</v>
       </c>
-      <c r="I104">
+      <c r="H104">
         <v>3940</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A105" s="1">
-        <v>103</v>
+    <row r="105" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B105">
+        <v>358469.67</v>
       </c>
       <c r="C105">
-        <v>358469.67</v>
+        <v>0</v>
       </c>
       <c r="D105">
-        <v>0</v>
+        <v>2398989.33</v>
       </c>
       <c r="E105">
-        <v>2398989.33</v>
+        <v>2757459</v>
       </c>
       <c r="F105">
-        <v>2757459</v>
-      </c>
-      <c r="G105">
         <v>404</v>
       </c>
-      <c r="H105" t="s">
+      <c r="G105" t="s">
         <v>239</v>
       </c>
-      <c r="I105">
+      <c r="H105">
         <v>3943</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A106" s="1">
-        <v>104</v>
+    <row r="106" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B106">
+        <v>609601.59</v>
       </c>
       <c r="C106">
-        <v>609601.59</v>
+        <v>0</v>
       </c>
       <c r="D106">
-        <v>0</v>
+        <v>4079641.41</v>
       </c>
       <c r="E106">
-        <v>4079641.41</v>
+        <v>4689243</v>
       </c>
       <c r="F106">
-        <v>4689243</v>
-      </c>
-      <c r="G106">
         <v>409</v>
       </c>
-      <c r="H106" t="s">
+      <c r="G106" t="s">
         <v>239</v>
       </c>
-      <c r="I106">
+      <c r="H106">
         <v>3975</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A107" s="1">
-        <v>105</v>
+    <row r="107" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B107">
+        <v>873637.94</v>
       </c>
       <c r="C107">
-        <v>873637.94</v>
+        <v>0</v>
       </c>
       <c r="D107">
-        <v>0</v>
+        <v>5366633.0599999996</v>
       </c>
       <c r="E107">
-        <v>5366633.0599999996</v>
+        <v>6240271</v>
       </c>
       <c r="F107">
-        <v>6240271</v>
-      </c>
-      <c r="G107">
         <v>408</v>
       </c>
-      <c r="H107" t="s">
+      <c r="G107" t="s">
         <v>239</v>
       </c>
-      <c r="I107">
+      <c r="H107">
         <v>3976</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A108" s="1">
-        <v>106</v>
+    <row r="108" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B108">
+        <v>1834151.34</v>
       </c>
       <c r="C108">
-        <v>1834151.34</v>
+        <v>0</v>
       </c>
       <c r="D108">
-        <v>0</v>
+        <v>11266929.66</v>
       </c>
       <c r="E108">
-        <v>11266929.66</v>
+        <v>13101081</v>
       </c>
       <c r="F108">
-        <v>13101081</v>
-      </c>
-      <c r="G108">
         <v>404</v>
       </c>
-      <c r="H108" t="s">
+      <c r="G108" t="s">
         <v>239</v>
       </c>
-      <c r="I108">
+      <c r="H108">
         <v>3979</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A109" s="1">
-        <v>107</v>
+    <row r="109" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B109">
+        <v>2340310.7000000002</v>
       </c>
       <c r="C109">
-        <v>2340310.7000000002</v>
+        <v>0</v>
       </c>
       <c r="D109">
-        <v>0</v>
+        <v>14376194.300000001</v>
       </c>
       <c r="E109">
-        <v>14376194.300000001</v>
+        <v>16716505</v>
       </c>
       <c r="F109">
-        <v>16716505</v>
-      </c>
-      <c r="G109">
         <v>408</v>
       </c>
-      <c r="H109" t="s">
+      <c r="G109" t="s">
         <v>239</v>
       </c>
-      <c r="I109">
+      <c r="H109">
         <v>3980</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A110" s="1">
-        <v>108</v>
+    <row r="110" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B110">
+        <v>1568890.82</v>
       </c>
       <c r="C110">
-        <v>1568890.82</v>
+        <v>0</v>
       </c>
       <c r="D110">
-        <v>0</v>
+        <v>9637472.0999999996</v>
       </c>
       <c r="E110">
-        <v>9637472.0999999996</v>
+        <v>11206362.92</v>
       </c>
       <c r="F110">
-        <v>11206362.92</v>
-      </c>
-      <c r="G110">
         <v>406</v>
       </c>
-      <c r="H110" t="s">
+      <c r="G110" t="s">
         <v>239</v>
       </c>
-      <c r="I110">
+      <c r="H110">
         <v>3983</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A111" s="1">
-        <v>109</v>
+    <row r="111" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B111">
+        <v>518839.72</v>
       </c>
       <c r="C111">
-        <v>518839.72</v>
+        <v>0</v>
       </c>
       <c r="D111">
-        <v>0</v>
+        <v>3187158.28</v>
       </c>
       <c r="E111">
-        <v>3187158.28</v>
+        <v>3705998</v>
       </c>
       <c r="F111">
-        <v>3705998</v>
-      </c>
-      <c r="G111">
         <v>405</v>
       </c>
-      <c r="H111" t="s">
+      <c r="G111" t="s">
         <v>239</v>
       </c>
-      <c r="I111">
+      <c r="H111">
         <v>3982</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A112" s="1">
-        <v>110</v>
+    <row r="112" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B112">
+        <v>2167640</v>
       </c>
       <c r="C112">
-        <v>2167640</v>
+        <v>0</v>
       </c>
       <c r="D112">
-        <v>0</v>
+        <v>13315506</v>
       </c>
       <c r="E112">
-        <v>13315506</v>
+        <v>15483146</v>
       </c>
       <c r="F112">
-        <v>15483146</v>
-      </c>
-      <c r="G112">
         <v>406</v>
       </c>
-      <c r="H112" t="s">
+      <c r="G112" t="s">
         <v>239</v>
       </c>
-      <c r="I112">
+      <c r="H112">
         <v>3984</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A113" s="1">
-        <v>111</v>
+    <row r="113" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B113">
+        <v>676010.20000000007</v>
       </c>
       <c r="C113">
-        <v>676010.20000000007</v>
+        <v>0</v>
       </c>
       <c r="D113">
-        <v>0</v>
+        <v>4152632.68</v>
       </c>
       <c r="E113">
-        <v>4152632.68</v>
+        <v>4828642.88</v>
       </c>
       <c r="F113">
-        <v>4828642.88</v>
-      </c>
-      <c r="G113">
         <v>409</v>
       </c>
-      <c r="H113" t="s">
+      <c r="G113" t="s">
         <v>239</v>
       </c>
-      <c r="I113">
+      <c r="H113">
         <v>3985</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A114" s="1">
-        <v>112</v>
+    <row r="114" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B114">
+        <v>51298.52</v>
       </c>
       <c r="C114">
-        <v>51298.52</v>
+        <v>0</v>
       </c>
       <c r="D114">
-        <v>0</v>
+        <v>315119.45</v>
       </c>
       <c r="E114">
-        <v>315119.45</v>
+        <v>366417.97</v>
       </c>
       <c r="F114">
-        <v>366417.97</v>
-      </c>
-      <c r="G114">
         <v>402</v>
       </c>
-      <c r="H114" t="s">
+      <c r="G114" t="s">
         <v>239</v>
       </c>
-      <c r="I114">
+      <c r="H114">
         <v>3986</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A115" s="1">
-        <v>113</v>
+    <row r="115" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B115">
+        <v>2884.54</v>
       </c>
       <c r="C115">
-        <v>2884.54</v>
+        <v>0</v>
       </c>
       <c r="D115">
-        <v>0</v>
+        <v>17719.310000000001</v>
       </c>
       <c r="E115">
-        <v>17719.310000000001</v>
+        <v>20603.849999999999</v>
       </c>
       <c r="F115">
-        <v>20603.849999999999</v>
-      </c>
-      <c r="G115">
         <v>404</v>
       </c>
-      <c r="H115" t="s">
+      <c r="G115" t="s">
         <v>239</v>
       </c>
-      <c r="I115">
+      <c r="H115">
         <v>3986</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A116" s="1">
-        <v>114</v>
+    <row r="116" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B116">
+        <v>543799.64</v>
       </c>
       <c r="C116">
-        <v>543799.64</v>
+        <v>0</v>
       </c>
       <c r="D116">
-        <v>0</v>
+        <v>3340483.54</v>
       </c>
       <c r="E116">
-        <v>3340483.54</v>
+        <v>3884283.18</v>
       </c>
       <c r="F116">
-        <v>3884283.18</v>
-      </c>
-      <c r="G116">
         <v>409</v>
       </c>
-      <c r="H116" t="s">
+      <c r="G116" t="s">
         <v>239</v>
       </c>
-      <c r="I116">
+      <c r="H116">
         <v>3986</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A117" s="1">
-        <v>115</v>
+    <row r="117" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B117">
+        <v>519371.58</v>
       </c>
       <c r="C117">
-        <v>519371.58</v>
+        <v>0</v>
       </c>
       <c r="D117">
-        <v>0</v>
+        <v>3475794</v>
       </c>
       <c r="E117">
-        <v>3475794</v>
+        <v>3995165.58</v>
       </c>
       <c r="F117">
-        <v>3995165.58</v>
-      </c>
-      <c r="G117">
         <v>404</v>
       </c>
-      <c r="H117" t="s">
+      <c r="G117" t="s">
         <v>239</v>
       </c>
-      <c r="I117">
+      <c r="H117">
         <v>3990</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A118" s="1">
-        <v>116</v>
+    <row r="118" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B118">
+        <v>1048318.64</v>
       </c>
       <c r="C118">
-        <v>1048318.64</v>
+        <v>0</v>
       </c>
       <c r="D118">
-        <v>0</v>
+        <v>7022996.3200000003</v>
       </c>
       <c r="E118">
-        <v>7022996.3200000003</v>
+        <v>8071314.96</v>
       </c>
       <c r="F118">
-        <v>8071314.96</v>
-      </c>
-      <c r="G118">
         <v>404</v>
       </c>
-      <c r="H118" t="s">
+      <c r="G118" t="s">
         <v>239</v>
       </c>
-      <c r="I118">
+      <c r="H118">
         <v>4037</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A119" s="1">
-        <v>117</v>
+    <row r="119" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B119">
+        <v>602645.49</v>
       </c>
       <c r="C119">
-        <v>602645.49</v>
+        <v>0</v>
       </c>
       <c r="D119">
-        <v>0</v>
+        <v>4025763.56</v>
       </c>
       <c r="E119">
-        <v>4025763.56</v>
+        <v>4628409.05</v>
       </c>
       <c r="F119">
-        <v>4628409.05</v>
-      </c>
-      <c r="G119">
         <v>409</v>
       </c>
-      <c r="H119" t="s">
+      <c r="G119" t="s">
         <v>239</v>
       </c>
-      <c r="I119">
+      <c r="H119">
         <v>4037</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A120" s="1">
-        <v>118</v>
+    <row r="120" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B120">
+        <v>621163.76</v>
       </c>
       <c r="C120">
-        <v>621163.76</v>
+        <v>0</v>
       </c>
       <c r="D120">
-        <v>0</v>
+        <v>3815720.24</v>
       </c>
       <c r="E120">
-        <v>3815720.24</v>
+        <v>4436884</v>
       </c>
       <c r="F120">
-        <v>4436884</v>
-      </c>
-      <c r="G120">
         <v>404</v>
       </c>
-      <c r="H120" t="s">
+      <c r="G120" t="s">
         <v>239</v>
       </c>
-      <c r="I120">
+      <c r="H120">
         <v>4030</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A121" s="1">
-        <v>119</v>
+    <row r="121" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B121">
+        <v>68774.16</v>
       </c>
       <c r="C121">
-        <v>68774.16</v>
+        <v>0</v>
       </c>
       <c r="D121">
-        <v>0</v>
+        <v>422469.83</v>
       </c>
       <c r="E121">
-        <v>422469.83</v>
+        <v>491243.99</v>
       </c>
       <c r="F121">
-        <v>491243.99</v>
-      </c>
-      <c r="G121">
         <v>402</v>
       </c>
-      <c r="H121" t="s">
+      <c r="G121" t="s">
         <v>239</v>
       </c>
-      <c r="I121">
+      <c r="H121">
         <v>4036</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A122" s="1">
-        <v>120</v>
+    <row r="122" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B122">
+        <v>2794367.94</v>
       </c>
       <c r="C122">
-        <v>2794367.94</v>
+        <v>0</v>
       </c>
       <c r="D122">
-        <v>0</v>
+        <v>17165403.07</v>
       </c>
       <c r="E122">
-        <v>17165403.07</v>
+        <v>19959771.010000002</v>
       </c>
       <c r="F122">
-        <v>19959771.010000002</v>
-      </c>
-      <c r="G122">
         <v>404</v>
       </c>
-      <c r="H122" t="s">
+      <c r="G122" t="s">
         <v>239</v>
       </c>
-      <c r="I122">
+      <c r="H122">
         <v>4036</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A123" s="1">
-        <v>121</v>
+    <row r="123" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B123">
+        <v>1903587.6</v>
       </c>
       <c r="C123">
-        <v>1903587.6</v>
+        <v>0</v>
       </c>
       <c r="D123">
-        <v>0</v>
+        <v>11693466.710000001</v>
       </c>
       <c r="E123">
-        <v>11693466.710000001</v>
+        <v>13597054.310000001</v>
       </c>
       <c r="F123">
-        <v>13597054.310000001</v>
-      </c>
-      <c r="G123">
         <v>402</v>
       </c>
-      <c r="H123" t="s">
+      <c r="G123" t="s">
         <v>239</v>
       </c>
-      <c r="I123">
+      <c r="H123">
         <v>3991</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A124" s="1">
-        <v>122</v>
+    <row r="124" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B124">
+        <v>455043.5</v>
       </c>
       <c r="C124">
-        <v>455043.5</v>
+        <v>0</v>
       </c>
       <c r="D124">
-        <v>0</v>
+        <v>2795267.19</v>
       </c>
       <c r="E124">
-        <v>2795267.19</v>
+        <v>3250310.69</v>
       </c>
       <c r="F124">
-        <v>3250310.69</v>
-      </c>
-      <c r="G124">
         <v>409</v>
       </c>
-      <c r="H124" t="s">
+      <c r="G124" t="s">
         <v>239</v>
       </c>
-      <c r="I124">
+      <c r="H124">
         <v>3991</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A125" s="1">
-        <v>123</v>
+    <row r="125" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B125">
+        <v>1635373.04</v>
       </c>
       <c r="C125">
-        <v>1635373.04</v>
+        <v>0</v>
       </c>
       <c r="D125">
-        <v>0</v>
+        <v>10045862.960000001</v>
       </c>
       <c r="E125">
-        <v>10045862.960000001</v>
+        <v>11681236</v>
       </c>
       <c r="F125">
-        <v>11681236</v>
-      </c>
-      <c r="G125">
         <v>407</v>
       </c>
-      <c r="H125" t="s">
+      <c r="G125" t="s">
         <v>239</v>
       </c>
-      <c r="I125">
+      <c r="H125">
         <v>4034</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A126" s="1">
-        <v>124</v>
+    <row r="126" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B126">
+        <v>537107.19999999995</v>
       </c>
       <c r="C126">
-        <v>537107.19999999995</v>
+        <v>0</v>
       </c>
       <c r="D126">
-        <v>0</v>
+        <v>3299372.8</v>
       </c>
       <c r="E126">
-        <v>3299372.8</v>
+        <v>3836480</v>
       </c>
       <c r="F126">
-        <v>3836480</v>
-      </c>
-      <c r="G126">
         <v>408</v>
       </c>
-      <c r="H126" t="s">
+      <c r="G126" t="s">
         <v>239</v>
       </c>
-      <c r="I126">
+      <c r="H126">
         <v>4038</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A127" s="1">
-        <v>125</v>
+    <row r="127" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B127">
+        <v>1507331.46</v>
       </c>
       <c r="C127">
-        <v>1507331.46</v>
+        <v>0</v>
       </c>
       <c r="D127">
-        <v>0</v>
+        <v>9259321.8200000003</v>
       </c>
       <c r="E127">
-        <v>9259321.8200000003</v>
+        <v>10766653.279999999</v>
       </c>
       <c r="F127">
-        <v>10766653.279999999</v>
-      </c>
-      <c r="G127">
         <v>404</v>
       </c>
-      <c r="H127" t="s">
+      <c r="G127" t="s">
         <v>239</v>
       </c>
-      <c r="I127">
+      <c r="H127">
         <v>3995</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A128" s="1">
-        <v>126</v>
+    <row r="128" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B128">
+        <v>705001.74</v>
       </c>
       <c r="C128">
-        <v>705001.74</v>
+        <v>0</v>
       </c>
       <c r="D128">
-        <v>0</v>
+        <v>4330724.9800000004</v>
       </c>
       <c r="E128">
-        <v>4330724.9800000004</v>
+        <v>5035726.7200000007</v>
       </c>
       <c r="F128">
-        <v>5035726.7200000007</v>
-      </c>
-      <c r="G128">
         <v>409</v>
       </c>
-      <c r="H128" t="s">
+      <c r="G128" t="s">
         <v>239</v>
       </c>
-      <c r="I128">
+      <c r="H128">
         <v>3995</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A129" s="1">
-        <v>127</v>
+    <row r="129" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B129">
+        <v>547239.29</v>
       </c>
       <c r="C129">
-        <v>547239.29</v>
+        <v>0</v>
       </c>
       <c r="D129">
-        <v>0</v>
+        <v>3662293.71</v>
       </c>
       <c r="E129">
-        <v>3662293.71</v>
+        <v>4209533</v>
       </c>
       <c r="F129">
-        <v>4209533</v>
-      </c>
-      <c r="G129">
         <v>411</v>
       </c>
-      <c r="H129" t="s">
+      <c r="G129" t="s">
         <v>239</v>
       </c>
-      <c r="I129">
+      <c r="H129">
         <v>4031</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A130" s="1">
-        <v>128</v>
+    <row r="130" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B130">
+        <v>152913.96</v>
       </c>
       <c r="C130">
-        <v>152913.96</v>
+        <v>0</v>
       </c>
       <c r="D130">
-        <v>0</v>
+        <v>939328.61</v>
       </c>
       <c r="E130">
-        <v>939328.61</v>
+        <v>1092242.57</v>
       </c>
       <c r="F130">
-        <v>1092242.57</v>
-      </c>
-      <c r="G130">
         <v>404</v>
       </c>
-      <c r="H130" t="s">
+      <c r="G130" t="s">
         <v>239</v>
       </c>
-      <c r="I130">
+      <c r="H130">
         <v>4021</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A131" s="1">
-        <v>129</v>
+    <row r="131" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B131">
+        <v>919237.26</v>
       </c>
       <c r="C131">
-        <v>919237.26</v>
+        <v>0</v>
       </c>
       <c r="D131">
-        <v>0</v>
+        <v>5646743.1699999999</v>
       </c>
       <c r="E131">
-        <v>5646743.1699999999</v>
+        <v>6565980.4299999997</v>
       </c>
       <c r="F131">
-        <v>6565980.4299999997</v>
-      </c>
-      <c r="G131">
         <v>405</v>
       </c>
-      <c r="H131" t="s">
+      <c r="G131" t="s">
         <v>239</v>
       </c>
-      <c r="I131">
+      <c r="H131">
         <v>4021</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A132" s="1">
-        <v>130</v>
+    <row r="132" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B132">
+        <v>360480.25</v>
       </c>
       <c r="C132">
-        <v>360480.25</v>
+        <v>0</v>
       </c>
       <c r="D132">
-        <v>0</v>
+        <v>2412444.75</v>
       </c>
       <c r="E132">
-        <v>2412444.75</v>
+        <v>2772925</v>
       </c>
       <c r="F132">
-        <v>2772925</v>
-      </c>
-      <c r="G132">
         <v>405</v>
       </c>
-      <c r="H132" t="s">
+      <c r="G132" t="s">
         <v>239</v>
       </c>
-      <c r="I132">
+      <c r="H132">
         <v>4010</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A133" s="1">
-        <v>131</v>
+    <row r="133" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B133">
+        <v>254904.63</v>
       </c>
       <c r="C133">
-        <v>254904.63</v>
+        <v>0</v>
       </c>
       <c r="D133">
-        <v>0</v>
+        <v>1565842.72</v>
       </c>
       <c r="E133">
-        <v>1565842.72</v>
+        <v>1820747.35</v>
       </c>
       <c r="F133">
-        <v>1820747.35</v>
-      </c>
-      <c r="G133">
         <v>404</v>
       </c>
-      <c r="H133" t="s">
+      <c r="G133" t="s">
         <v>239</v>
       </c>
-      <c r="I133">
+      <c r="H133">
         <v>4039</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A134" s="1">
-        <v>132</v>
+    <row r="134" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B134">
+        <v>169568.04</v>
       </c>
       <c r="C134">
-        <v>169568.04</v>
+        <v>0</v>
       </c>
       <c r="D134">
-        <v>0</v>
+        <v>1041632.22</v>
       </c>
       <c r="E134">
-        <v>1041632.22</v>
+        <v>1211200.26</v>
       </c>
       <c r="F134">
-        <v>1211200.26</v>
-      </c>
-      <c r="G134">
         <v>405</v>
       </c>
-      <c r="H134" t="s">
+      <c r="G134" t="s">
         <v>239</v>
       </c>
-      <c r="I134">
+      <c r="H134">
         <v>4039</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A135" s="1">
-        <v>133</v>
+    <row r="135" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B135">
+        <v>3063.68</v>
       </c>
       <c r="C135">
-        <v>3063.68</v>
+        <v>0</v>
       </c>
       <c r="D135">
-        <v>0</v>
+        <v>18819.73</v>
       </c>
       <c r="E135">
-        <v>18819.73</v>
+        <v>21883.41</v>
       </c>
       <c r="F135">
-        <v>21883.41</v>
-      </c>
-      <c r="G135">
         <v>409</v>
       </c>
-      <c r="H135" t="s">
+      <c r="G135" t="s">
         <v>239</v>
       </c>
-      <c r="I135">
+      <c r="H135">
         <v>4039</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A136" s="1">
-        <v>134</v>
+    <row r="136" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B136">
+        <v>738001.16</v>
       </c>
       <c r="C136">
-        <v>738001.16</v>
+        <v>0</v>
       </c>
       <c r="D136">
-        <v>0</v>
+        <v>4938930.84</v>
       </c>
       <c r="E136">
-        <v>4938930.84</v>
+        <v>5676932</v>
       </c>
       <c r="F136">
-        <v>5676932</v>
-      </c>
-      <c r="G136">
         <v>409</v>
       </c>
-      <c r="H136" t="s">
+      <c r="G136" t="s">
         <v>239</v>
       </c>
-      <c r="I136">
+      <c r="H136">
         <v>4035</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A137" s="1">
-        <v>135</v>
+    <row r="137" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B137">
+        <v>139782.47</v>
       </c>
       <c r="C137">
-        <v>139782.47</v>
+        <v>0</v>
       </c>
       <c r="D137">
-        <v>0</v>
+        <v>858663.75</v>
       </c>
       <c r="E137">
-        <v>858663.75</v>
+        <v>998446.22</v>
       </c>
       <c r="F137">
-        <v>998446.22</v>
-      </c>
-      <c r="G137">
         <v>404</v>
       </c>
-      <c r="H137" t="s">
+      <c r="G137" t="s">
         <v>239</v>
       </c>
-      <c r="I137">
+      <c r="H137">
         <v>4033</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A138" s="1">
-        <v>136</v>
+    <row r="138" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B138">
+        <v>134681.23000000001</v>
       </c>
       <c r="C138">
-        <v>134681.23000000001</v>
+        <v>0</v>
       </c>
       <c r="D138">
-        <v>0</v>
+        <v>827327.55</v>
       </c>
       <c r="E138">
-        <v>827327.55</v>
+        <v>962008.78</v>
       </c>
       <c r="F138">
-        <v>962008.78</v>
-      </c>
-      <c r="G138">
         <v>409</v>
       </c>
-      <c r="H138" t="s">
+      <c r="G138" t="s">
         <v>239</v>
       </c>
-      <c r="I138">
+      <c r="H138">
         <v>4033</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A139" s="1">
-        <v>137</v>
+    <row r="139" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B139">
+        <v>1101691.92</v>
       </c>
       <c r="C139">
-        <v>1101691.92</v>
+        <v>0</v>
       </c>
       <c r="D139">
-        <v>0</v>
+        <v>6767346.0800000001</v>
       </c>
       <c r="E139">
-        <v>6767346.0800000001</v>
+        <v>7869038</v>
       </c>
       <c r="F139">
-        <v>7869038</v>
-      </c>
-      <c r="G139">
         <v>405</v>
       </c>
-      <c r="H139" t="s">
+      <c r="G139" t="s">
         <v>239</v>
       </c>
-      <c r="I139">
+      <c r="H139">
         <v>4029</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A140" s="1">
-        <v>138</v>
+    <row r="140" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B140">
+        <v>111409.39</v>
       </c>
       <c r="C140">
-        <v>111409.39</v>
+        <v>0</v>
       </c>
       <c r="D140">
-        <v>0</v>
+        <v>684371.95</v>
       </c>
       <c r="E140">
-        <v>684371.95</v>
+        <v>795781.34</v>
       </c>
       <c r="F140">
-        <v>795781.34</v>
-      </c>
-      <c r="G140">
         <v>402</v>
       </c>
-      <c r="H140" t="s">
+      <c r="G140" t="s">
         <v>239</v>
       </c>
-      <c r="I140">
+      <c r="H140">
         <v>4032</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A141" s="1">
-        <v>139</v>
+    <row r="141" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B141">
+        <v>145566.37</v>
       </c>
       <c r="C141">
-        <v>145566.37</v>
+        <v>0</v>
       </c>
       <c r="D141">
-        <v>0</v>
+        <v>894193.39</v>
       </c>
       <c r="E141">
-        <v>894193.39</v>
+        <v>1039759.76</v>
       </c>
       <c r="F141">
-        <v>1039759.76</v>
-      </c>
-      <c r="G141">
         <v>404</v>
       </c>
-      <c r="H141" t="s">
+      <c r="G141" t="s">
         <v>239</v>
       </c>
-      <c r="I141">
+      <c r="H141">
         <v>4032</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A142" s="1">
-        <v>140</v>
+    <row r="142" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B142">
+        <v>723530.63</v>
       </c>
       <c r="C142">
-        <v>723530.63</v>
+        <v>0</v>
       </c>
       <c r="D142">
-        <v>0</v>
+        <v>4444545.28</v>
       </c>
       <c r="E142">
-        <v>4444545.28</v>
+        <v>5168075.91</v>
       </c>
       <c r="F142">
-        <v>5168075.91</v>
-      </c>
-      <c r="G142">
         <v>409</v>
       </c>
-      <c r="H142" t="s">
+      <c r="G142" t="s">
         <v>239</v>
       </c>
-      <c r="I142">
+      <c r="H142">
         <v>4032</v>
       </c>
     </row>
@@ -52674,7 +52259,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S94"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>

</xml_diff>